<commit_message>
Added feature to OdkPrompt to extract question number from question label. Also did the following. - Some modifications to OdkFormTest.xlsx for the purposes of this. - Minor de-linting.
</commit_message>
<xml_diff>
--- a/test/files/OdkFormTest.xlsx
+++ b/test/files/OdkFormTest.xlsx
@@ -1038,13 +1038,7 @@
     <t>ever_birth</t>
   </si>
   <si>
-    <t>200. Now I would like to ask about all the births you have had during your life. Have you ever given birth?</t>
-  </si>
-  <si>
     <t>children_living</t>
-  </si>
-  <si>
-    <t>201a. Do you have any sons or daughters to whom you have given birth who are now living with you?</t>
   </si>
   <si>
     <t>205. When was your FIRST birth?</t>
@@ -1775,6 +1769,12 @@
   </si>
   <si>
     <t>ppp_input::English</t>
+  </si>
+  <si>
+    <t>200.  Now I would like to ask about all the births you have had during your life. Have you ever given birth?</t>
+  </si>
+  <si>
+    <t>201a.       Do you have any sons or daughters to whom you have given birth who are now living with you?</t>
   </si>
 </sst>
 </file>
@@ -4479,7 +4479,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13" customHeight="1" x14ac:dyDescent="0"/>
@@ -4558,133 +4558,133 @@
         <v>12</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="Q1" s="33" t="s">
+        <v>402</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="S1" s="33" t="s">
         <v>404</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="T1" s="33" t="s">
         <v>405</v>
       </c>
-      <c r="S1" s="33" t="s">
+      <c r="U1" s="33" t="s">
         <v>406</v>
       </c>
-      <c r="T1" s="33" t="s">
+      <c r="V1" s="33" t="s">
         <v>407</v>
       </c>
-      <c r="U1" s="33" t="s">
+      <c r="W1" s="33" t="s">
         <v>408</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="X1" s="33" t="s">
         <v>409</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="Y1" s="33" t="s">
         <v>410</v>
       </c>
-      <c r="X1" s="33" t="s">
+      <c r="Z1" s="33" t="s">
         <v>411</v>
       </c>
-      <c r="Y1" s="33" t="s">
+      <c r="AA1" s="33" t="s">
         <v>412</v>
       </c>
-      <c r="Z1" s="33" t="s">
+      <c r="AB1" s="33" t="s">
         <v>413</v>
       </c>
-      <c r="AA1" s="33" t="s">
+      <c r="AC1" s="33" t="s">
         <v>414</v>
       </c>
-      <c r="AB1" s="33" t="s">
+      <c r="AD1" s="33" t="s">
         <v>415</v>
       </c>
-      <c r="AC1" s="33" t="s">
+      <c r="AE1" s="33" t="s">
         <v>416</v>
       </c>
-      <c r="AD1" s="33" t="s">
+      <c r="AF1" s="33" t="s">
         <v>417</v>
       </c>
-      <c r="AE1" s="33" t="s">
+      <c r="AG1" s="33" t="s">
         <v>418</v>
       </c>
-      <c r="AF1" s="33" t="s">
+      <c r="AH1" s="33" t="s">
         <v>419</v>
       </c>
-      <c r="AG1" s="33" t="s">
+      <c r="AI1" s="33" t="s">
         <v>420</v>
       </c>
-      <c r="AH1" s="33" t="s">
+      <c r="AJ1" s="33" t="s">
         <v>421</v>
       </c>
-      <c r="AI1" s="33" t="s">
+      <c r="AK1" s="33" t="s">
         <v>422</v>
       </c>
-      <c r="AJ1" s="33" t="s">
+      <c r="AL1" s="33" t="s">
         <v>423</v>
       </c>
-      <c r="AK1" s="33" t="s">
+      <c r="AM1" s="33" t="s">
         <v>424</v>
       </c>
-      <c r="AL1" s="33" t="s">
+      <c r="AN1" s="33" t="s">
         <v>425</v>
       </c>
-      <c r="AM1" s="33" t="s">
-        <v>426</v>
-      </c>
-      <c r="AN1" s="33" t="s">
-        <v>427</v>
-      </c>
       <c r="AO1" s="33" t="s">
+        <v>524</v>
+      </c>
+      <c r="AP1" s="33" t="s">
+        <v>525</v>
+      </c>
+      <c r="AQ1" s="33" t="s">
         <v>526</v>
       </c>
-      <c r="AP1" s="33" t="s">
+      <c r="AR1" s="33" t="s">
         <v>527</v>
       </c>
-      <c r="AQ1" s="33" t="s">
+      <c r="AS1" s="33" t="s">
         <v>528</v>
       </c>
-      <c r="AR1" s="33" t="s">
+      <c r="AT1" s="33" t="s">
         <v>529</v>
       </c>
-      <c r="AS1" s="33" t="s">
+      <c r="AU1" s="33" t="s">
         <v>530</v>
       </c>
-      <c r="AT1" s="33" t="s">
+      <c r="AV1" s="33" t="s">
         <v>531</v>
       </c>
-      <c r="AU1" s="33" t="s">
-        <v>532</v>
-      </c>
-      <c r="AV1" s="33" t="s">
-        <v>533</v>
-      </c>
       <c r="AX1" s="39" t="s">
+        <v>569</v>
+      </c>
+      <c r="AY1" s="39" t="s">
+        <v>578</v>
+      </c>
+      <c r="AZ1" s="33" t="s">
+        <v>570</v>
+      </c>
+      <c r="BA1" s="33" t="s">
         <v>571</v>
       </c>
-      <c r="AY1" s="39" t="s">
-        <v>580</v>
-      </c>
-      <c r="AZ1" s="33" t="s">
+      <c r="BB1" s="33" t="s">
         <v>572</v>
       </c>
-      <c r="BA1" s="33" t="s">
+      <c r="BC1" s="33" t="s">
         <v>573</v>
       </c>
-      <c r="BB1" s="33" t="s">
+      <c r="BD1" s="33" t="s">
         <v>574</v>
       </c>
-      <c r="BC1" s="33" t="s">
+      <c r="BE1" s="33" t="s">
         <v>575</v>
       </c>
-      <c r="BD1" s="33" t="s">
+      <c r="BF1" s="33" t="s">
         <v>576</v>
       </c>
-      <c r="BE1" s="33" t="s">
+      <c r="BG1" s="33" t="s">
         <v>577</v>
-      </c>
-      <c r="BF1" s="33" t="s">
-        <v>578</v>
-      </c>
-      <c r="BG1" s="33" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="2" spans="1:59" s="12" customFormat="1" ht="13" customHeight="1">
@@ -4695,7 +4695,7 @@
         <v>336</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>337</v>
+        <v>579</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -4714,28 +4714,28 @@
       <c r="N2" s="10"/>
       <c r="O2" s="16"/>
       <c r="Q2" s="10" t="s">
+        <v>519</v>
+      </c>
+      <c r="R2" s="10" t="s">
+        <v>512</v>
+      </c>
+      <c r="S2" s="10" t="s">
+        <v>510</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>508</v>
+      </c>
+      <c r="U2" s="10" t="s">
         <v>521</v>
       </c>
-      <c r="R2" s="10" t="s">
+      <c r="V2" s="10" t="s">
+        <v>517</v>
+      </c>
+      <c r="W2" s="10" t="s">
+        <v>522</v>
+      </c>
+      <c r="X2" s="10" t="s">
         <v>514</v>
-      </c>
-      <c r="S2" s="10" t="s">
-        <v>512</v>
-      </c>
-      <c r="T2" s="10" t="s">
-        <v>510</v>
-      </c>
-      <c r="U2" s="10" t="s">
-        <v>523</v>
-      </c>
-      <c r="V2" s="10" t="s">
-        <v>519</v>
-      </c>
-      <c r="W2" s="10" t="s">
-        <v>524</v>
-      </c>
-      <c r="X2" s="10" t="s">
-        <v>516</v>
       </c>
       <c r="Y2" s="33"/>
       <c r="Z2" s="33"/>
@@ -4769,7 +4769,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="35" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C3" s="35"/>
       <c r="D3" s="35"/>
@@ -4781,7 +4781,7 @@
       </c>
       <c r="I3" s="35"/>
       <c r="J3" s="35" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="K3" s="35"/>
       <c r="L3" s="35"/>
@@ -4800,13 +4800,13 @@
         <v>16</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D4" s="16" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
@@ -4820,52 +4820,52 @@
       <c r="N4" s="16"/>
       <c r="O4" s="10"/>
       <c r="Q4" s="33" t="s">
+        <v>499</v>
+      </c>
+      <c r="R4" s="33" t="s">
+        <v>497</v>
+      </c>
+      <c r="S4" s="33" t="s">
+        <v>500</v>
+      </c>
+      <c r="T4" s="33" t="s">
         <v>501</v>
       </c>
-      <c r="R4" s="33" t="s">
-        <v>499</v>
-      </c>
-      <c r="S4" s="33" t="s">
+      <c r="U4" s="33" t="s">
         <v>502</v>
       </c>
-      <c r="T4" s="33" t="s">
+      <c r="V4" s="33" t="s">
         <v>503</v>
       </c>
-      <c r="U4" s="33" t="s">
+      <c r="W4" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="X4" s="33" t="s">
         <v>504</v>
       </c>
-      <c r="V4" s="33" t="s">
-        <v>505</v>
-      </c>
-      <c r="W4" s="33" t="s">
-        <v>525</v>
-      </c>
-      <c r="X4" s="33" t="s">
-        <v>506</v>
-      </c>
       <c r="Y4" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="Z4" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AA4" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AB4" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AC4" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AD4" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AE4" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AF4" s="33" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="AG4" s="16" t="s">
         <v>24</v>
@@ -4904,13 +4904,13 @@
     </row>
     <row r="5" spans="1:59" s="36" customFormat="1" ht="13" customHeight="1">
       <c r="A5" s="38" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C5" s="35" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="D5" s="35"/>
       <c r="E5" s="35"/>
@@ -4919,7 +4919,7 @@
         <v>17</v>
       </c>
       <c r="H5" s="35" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="I5" s="35"/>
       <c r="J5" s="35"/>
@@ -4940,23 +4940,23 @@
         <v>22</v>
       </c>
       <c r="B6" s="35" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C6" s="35" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="D6" s="35"/>
       <c r="E6" s="35" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F6" s="35" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="35" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="I6" s="35" t="s">
         <v>23</v>
@@ -4979,7 +4979,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="35" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C7" s="35"/>
       <c r="D7" s="35"/>
@@ -5006,17 +5006,17 @@
         <v>19</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>27</v>
       </c>
       <c r="E8" s="10"/>
       <c r="F8" s="10" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>17</v>
@@ -5024,7 +5024,7 @@
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
       <c r="J8" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="K8" s="10"/>
       <c r="L8" s="10"/>
@@ -5032,52 +5032,52 @@
       <c r="N8" s="10"/>
       <c r="O8" s="16"/>
       <c r="Q8" s="10" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="R8" s="10" t="s">
+        <v>507</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>511</v>
+      </c>
+      <c r="T8" s="10" t="s">
         <v>509</v>
       </c>
-      <c r="S8" s="10" t="s">
-        <v>513</v>
-      </c>
-      <c r="T8" s="10" t="s">
-        <v>511</v>
-      </c>
       <c r="U8" s="10" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="V8" s="10" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="W8" s="10" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="X8" s="10" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="Y8" s="33" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="Z8" s="33" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AA8" s="33" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AB8" s="33" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AC8" s="33" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AD8" s="33" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AE8" s="33" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AF8" s="33" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="AG8" s="10"/>
       <c r="AH8" s="10"/>
@@ -5103,10 +5103,10 @@
         <v>26</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>339</v>
+        <v>580</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -5117,7 +5117,7 @@
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
       <c r="J9" s="10" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -5125,28 +5125,28 @@
       <c r="N9" s="10"/>
       <c r="O9" s="16"/>
       <c r="Q9" s="33" t="s">
+        <v>494</v>
+      </c>
+      <c r="R9" s="33" t="s">
+        <v>491</v>
+      </c>
+      <c r="S9" s="33" t="s">
+        <v>495</v>
+      </c>
+      <c r="T9" s="33" t="s">
         <v>496</v>
       </c>
-      <c r="R9" s="33" t="s">
+      <c r="U9" s="33" t="s">
+        <v>498</v>
+      </c>
+      <c r="V9" s="33" t="s">
         <v>493</v>
       </c>
-      <c r="S9" s="33" t="s">
-        <v>497</v>
-      </c>
-      <c r="T9" s="33" t="s">
-        <v>498</v>
-      </c>
-      <c r="U9" s="33" t="s">
-        <v>500</v>
-      </c>
-      <c r="V9" s="33" t="s">
-        <v>495</v>
-      </c>
       <c r="W9" s="33" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="X9" s="33" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="Y9" s="33"/>
       <c r="Z9" s="33"/>
@@ -5218,31 +5218,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="E1" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>403</v>
+      </c>
+      <c r="G1" s="13" t="s">
         <v>404</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="H1" s="13" t="s">
         <v>405</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="I1" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="J1" s="13" t="s">
         <v>407</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="K1" s="13" t="s">
         <v>408</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>409</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>410</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="13" customHeight="1">
@@ -6027,31 +6027,31 @@
         <v>57</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="G24" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="J24" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="K24" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="L24" s="13" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
@@ -6059,34 +6059,34 @@
         <v>56</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="I25" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="J25" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="K25" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="L25" s="13" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
@@ -6094,34 +6094,34 @@
         <v>56</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="27" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
@@ -6129,34 +6129,34 @@
         <v>56</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="E27" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="G27" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="28" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
@@ -6164,34 +6164,34 @@
         <v>56</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="E28" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="G28" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="I28" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="J28" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="K28" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="L28" s="13" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="29" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
@@ -6199,34 +6199,34 @@
         <v>56</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="J29" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="K29" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="L29" s="13" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="30" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
@@ -6234,34 +6234,34 @@
         <v>56</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="J30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="K30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="31" spans="1:12" s="13" customFormat="1" ht="13" customHeight="1">
@@ -7021,151 +7021,151 @@
     </row>
     <row r="52" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A52" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B52" s="13" t="s">
         <v>93</v>
       </c>
       <c r="C52" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D52" s="13"/>
       <c r="E52" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G52" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="H52" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="I52" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="J52" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="K52" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="L52" s="15" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="53" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A53" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B53" s="13" t="s">
         <v>94</v>
       </c>
       <c r="C53" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="D53" s="13"/>
       <c r="E53" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="G53" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="H53" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="I53" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="J53" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K53" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="L53" s="15" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="54" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A54" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B54" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C54" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D54" s="13"/>
       <c r="E54" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G54" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H54" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="I54" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J54" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K54" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L54" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="55" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A55" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B55" s="13">
         <v>-88</v>
       </c>
       <c r="C55" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D55" s="13"/>
       <c r="E55" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G55" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H55" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I55" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J55" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K55" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L55" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="56" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A56" s="15" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B56" s="13">
         <v>-99</v>
@@ -7201,151 +7201,151 @@
     </row>
     <row r="57" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A57" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B57" s="13" t="s">
         <v>93</v>
       </c>
       <c r="C57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="D57" s="13"/>
       <c r="E57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="G57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="H57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="I57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="J57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="K57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="L57" s="15" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="58" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A58" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B58" s="13" t="s">
         <v>94</v>
       </c>
       <c r="C58" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D58" s="13"/>
       <c r="E58" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="F58" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G58" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="H58" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="I58" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="J58" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="K58" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="L58" s="15" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="59" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A59" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B59" s="13" t="s">
         <v>95</v>
       </c>
       <c r="C59" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D59" s="13"/>
       <c r="E59" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G59" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="H59" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="I59" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="J59" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="K59" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="L59" s="15" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="60" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A60" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B60" s="13">
         <v>-88</v>
       </c>
       <c r="C60" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="D60" s="13"/>
       <c r="E60" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G60" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="H60" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="I60" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="J60" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="K60" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="L60" s="15" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="61" spans="1:12" s="8" customFormat="1" ht="13" customHeight="1">
       <c r="A61" s="15" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B61" s="13">
         <v>-99</v>
@@ -7787,28 +7787,28 @@
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F73" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="G73" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="I73" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="J73" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="K73" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="L73" s="13" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="74" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -7823,28 +7823,28 @@
       </c>
       <c r="D74" s="12"/>
       <c r="E74" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F74" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="G74" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I74" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="J74" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="K74" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="L74" s="13" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
     </row>
     <row r="75" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -7859,28 +7859,28 @@
       </c>
       <c r="D75" s="12"/>
       <c r="E75" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F75" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G75" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I75" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J75" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="K75" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="L75" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="76" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -7967,28 +7967,28 @@
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F78" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G78" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I78" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J78" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="K78" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="L78" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="79" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8003,28 +8003,28 @@
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F79" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G79" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="I79" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="J79" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K79" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L79" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="80" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8039,28 +8039,28 @@
       </c>
       <c r="D80" s="12"/>
       <c r="E80" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F80" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G80" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I80" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J80" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="K80" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="L80" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="81" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8075,28 +8075,28 @@
       </c>
       <c r="D81" s="12"/>
       <c r="E81" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F81" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G81" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I81" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="J81" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="K81" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="L81" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="82" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8104,35 +8104,35 @@
         <v>112</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F82" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G82" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I82" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="J82" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="K82" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="L82" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="83" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8143,32 +8143,32 @@
         <v>301</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F83" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G83" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I83" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J83" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="K83" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="L83" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="84" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8183,28 +8183,28 @@
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F84" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G84" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="I84" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="J84" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="K84" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="L84" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="85" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8255,28 +8255,28 @@
       </c>
       <c r="D86" s="12"/>
       <c r="E86" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F86" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G86" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I86" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="J86" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="K86" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L86" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="87" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8291,28 +8291,28 @@
       </c>
       <c r="D87" s="12"/>
       <c r="E87" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F87" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G87" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I87" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J87" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="K87" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="L87" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="88" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8363,28 +8363,28 @@
       </c>
       <c r="D89" s="12"/>
       <c r="E89" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F89" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="G89" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I89" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="J89" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="K89" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="L89" s="13" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="90" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8471,28 +8471,28 @@
       </c>
       <c r="D92" s="12"/>
       <c r="E92" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="F92" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="G92" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I92" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="J92" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="K92" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="L92" s="13" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="93" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8507,28 +8507,28 @@
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="F93" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="G93" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="I93" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="J93" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="K93" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="L93" s="13" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="94" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8543,28 +8543,28 @@
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="F94" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="G94" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I94" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="J94" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="K94" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="L94" s="13" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="95" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8579,28 +8579,28 @@
       </c>
       <c r="D95" s="12"/>
       <c r="E95" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="F95" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="G95" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I95" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="J95" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="K95" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="L95" s="13" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="96" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8608,35 +8608,35 @@
         <v>237</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D96" s="12"/>
       <c r="E96" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F96" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="G96" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I96" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="J96" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="K96" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="L96" s="13" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
     </row>
     <row r="97" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8647,32 +8647,32 @@
         <v>301</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D97" s="12"/>
       <c r="E97" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F97" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="G97" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I97" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="J97" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="K97" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="L97" s="13" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
     </row>
     <row r="98" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8687,28 +8687,28 @@
       </c>
       <c r="D98" s="12"/>
       <c r="E98" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F98" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="G98" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="I98" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="J98" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="K98" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="L98" s="13" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
     </row>
     <row r="99" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8759,28 +8759,28 @@
       </c>
       <c r="D100" s="12"/>
       <c r="E100" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="F100" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="G100" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I100" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="J100" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="K100" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="L100" s="13" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
     </row>
     <row r="101" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8795,28 +8795,28 @@
       </c>
       <c r="D101" s="12"/>
       <c r="E101" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="F101" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="G101" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="H101" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I101" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="J101" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="K101" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="L101" s="13" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
     </row>
     <row r="102" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -8939,28 +8939,28 @@
       </c>
       <c r="D105" s="13"/>
       <c r="E105" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F105" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="G105" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="H105" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I105" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="J105" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="K105" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="L105" s="13" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="13" customHeight="1">
@@ -10415,28 +10415,28 @@
       </c>
       <c r="D146" s="13"/>
       <c r="E146" s="13" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="F146" s="13" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="G146" s="13" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="H146" s="13" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I146" s="13" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="J146" s="13" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="K146" s="13" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="L146" s="13" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
     </row>
     <row r="147" spans="1:12" ht="13" customHeight="1">
@@ -10735,32 +10735,32 @@
         <v>216</v>
       </c>
       <c r="C155" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D155" s="13"/>
       <c r="E155" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="F155" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="G155" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H155" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="I155" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="J155" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="K155" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="L155" s="13" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="156" spans="1:12" ht="13" customHeight="1">
@@ -10771,32 +10771,32 @@
         <v>217</v>
       </c>
       <c r="C156" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="D156" s="13"/>
       <c r="E156" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F156" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="G156" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H156" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="I156" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="J156" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="K156" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="L156" s="13" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="157" spans="1:12" ht="13" customHeight="1">
@@ -11524,35 +11524,35 @@
         <v>251</v>
       </c>
       <c r="B177" s="18" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C177" s="18" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="D177" s="31"/>
       <c r="E177" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="F177" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="G177" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H177" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="I177" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="J177" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="K177" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="L177" s="13" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
     </row>
     <row r="178" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11560,35 +11560,35 @@
         <v>251</v>
       </c>
       <c r="B178" s="18" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C178" s="18" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="D178" s="31"/>
       <c r="E178" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F178" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="G178" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H178" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="I178" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="J178" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="K178" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="L178" s="13" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="179" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11596,35 +11596,35 @@
         <v>251</v>
       </c>
       <c r="B179" s="18" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="C179" s="18" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="D179" s="31"/>
       <c r="E179" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="F179" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="G179" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H179" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="I179" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="J179" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="K179" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="L179" s="13" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="180" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11632,35 +11632,35 @@
         <v>251</v>
       </c>
       <c r="B180" s="18" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="C180" s="18" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="D180" s="31"/>
       <c r="E180" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="F180" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="G180" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H180" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="I180" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="J180" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="K180" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="L180" s="13" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
     </row>
     <row r="181" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11668,35 +11668,35 @@
         <v>251</v>
       </c>
       <c r="B181" s="18" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="C181" s="18" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="D181" s="31"/>
       <c r="E181" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="F181" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="G181" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="H181" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="I181" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="J181" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="K181" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="L181" s="13" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
     </row>
     <row r="182" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11704,35 +11704,35 @@
         <v>251</v>
       </c>
       <c r="B182" s="18" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C182" s="18" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="D182" s="31"/>
       <c r="E182" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="F182" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="G182" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H182" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="I182" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="J182" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="K182" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="L182" s="13" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
     </row>
     <row r="183" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11740,35 +11740,35 @@
         <v>251</v>
       </c>
       <c r="B183" s="18" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="C183" s="18" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="D183" s="31"/>
       <c r="E183" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="F183" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="G183" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H183" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="I183" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="J183" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="K183" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="L183" s="13" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row r="184" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11779,32 +11779,32 @@
         <v>252</v>
       </c>
       <c r="C184" s="18" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D184" s="31"/>
       <c r="E184" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="F184" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G184" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="H184" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="I184" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="J184" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="K184" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="L184" s="13" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="185" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11812,35 +11812,35 @@
         <v>251</v>
       </c>
       <c r="B185" s="18" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="C185" s="18" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="D185" s="31"/>
       <c r="E185" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="F185" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="G185" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H185" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="I185" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="J185" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="K185" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="L185" s="13" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
     </row>
     <row r="186" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11848,35 +11848,35 @@
         <v>251</v>
       </c>
       <c r="B186" s="18" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="C186" s="18" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="D186" s="31"/>
       <c r="E186" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="F186" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G186" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="H186" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I186" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="J186" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="K186" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="L186" s="13" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
     </row>
     <row r="187" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11884,35 +11884,35 @@
         <v>251</v>
       </c>
       <c r="B187" s="18" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="C187" s="18" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="D187" s="31"/>
       <c r="E187" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="F187" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="G187" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="H187" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I187" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="J187" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="K187" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="L187" s="13" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
     </row>
     <row r="188" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11920,35 +11920,35 @@
         <v>251</v>
       </c>
       <c r="B188" s="18" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="C188" s="18" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="D188" s="31"/>
       <c r="E188" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="F188" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="G188" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="H188" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I188" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="J188" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="K188" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="L188" s="13" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
     </row>
     <row r="189" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11956,35 +11956,35 @@
         <v>251</v>
       </c>
       <c r="B189" s="18" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="C189" s="18" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="D189" s="31"/>
       <c r="E189" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="F189" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="G189" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="H189" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I189" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="J189" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="K189" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="L189" s="13" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
     </row>
     <row r="190" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -11995,32 +11995,32 @@
         <v>253</v>
       </c>
       <c r="C190" s="18" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="D190" s="31"/>
       <c r="E190" s="13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F190" s="13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="G190" s="13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="H190" s="13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="I190" s="13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="J190" s="13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="K190" s="13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="L190" s="13" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
     </row>
     <row r="191" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
@@ -12133,115 +12133,115 @@
     </row>
     <row r="194" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A194" s="19" t="s">
+        <v>339</v>
+      </c>
+      <c r="B194" s="19" t="s">
+        <v>340</v>
+      </c>
+      <c r="C194" s="20" t="s">
         <v>341</v>
-      </c>
-      <c r="B194" s="19" t="s">
-        <v>342</v>
-      </c>
-      <c r="C194" s="20" t="s">
-        <v>343</v>
       </c>
       <c r="D194" s="19"/>
       <c r="E194" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="F194" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G194" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H194" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="I194" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="J194" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="K194" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="L194" s="20" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="195" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A195" s="21" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B195" s="21" t="s">
         <v>146</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D195" s="21"/>
       <c r="E195" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="F195" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="G195" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H195" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="I195" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="J195" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="K195" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="L195" s="3" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="196" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A196" s="21" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B196" s="21" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D196" s="21"/>
       <c r="E196" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="F196" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G196" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H196" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="I196" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="J196" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="K196" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="L196" s="3" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="197" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A197" s="21" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B197" s="21" t="s">
         <v>102</v>
@@ -12277,7 +12277,7 @@
     </row>
     <row r="198" spans="1:12" s="7" customFormat="1" ht="13" customHeight="1">
       <c r="A198" s="21" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="B198" s="21">
         <v>-99</v>
@@ -14113,151 +14113,151 @@
     </row>
     <row r="249" spans="1:12" ht="13" customHeight="1">
       <c r="A249" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B249" s="13">
         <v>1</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="D249" s="13"/>
       <c r="E249" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="F249" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="G249" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H249" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I249" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J249" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K249" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="L249" s="3" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
     </row>
     <row r="250" spans="1:12" ht="13" customHeight="1">
       <c r="A250" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B250" s="13">
         <v>2</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="D250" s="13"/>
       <c r="E250" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="F250" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="G250" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="H250" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I250" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="J250" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="K250" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="L250" s="3" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
     </row>
     <row r="251" spans="1:12" ht="13" customHeight="1">
       <c r="A251" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B251" s="13">
         <v>3</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="D251" s="13"/>
       <c r="E251" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="F251" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="G251" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="H251" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I251" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="J251" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="K251" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="L251" s="3" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
     </row>
     <row r="252" spans="1:12" ht="13" customHeight="1">
       <c r="A252" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B252" s="13">
         <v>4</v>
       </c>
       <c r="C252" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D252" s="13"/>
       <c r="E252" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F252" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="G252" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="H252" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I252" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="J252" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="K252" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="L252" s="3" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
     </row>
     <row r="253" spans="1:12" ht="13" customHeight="1">
       <c r="A253" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="B253" s="13">
         <v>-99</v>
@@ -14293,151 +14293,151 @@
     </row>
     <row r="254" spans="1:12" ht="13" customHeight="1">
       <c r="A254" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B254" s="13">
         <v>1</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="D254" s="13"/>
       <c r="E254" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F254" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="G254" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="H254" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I254" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="J254" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K254" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="L254" s="3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
     </row>
     <row r="255" spans="1:12" ht="13" customHeight="1">
       <c r="A255" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B255" s="13">
         <v>2</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="D255" s="13"/>
       <c r="E255" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="F255" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="G255" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="H255" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I255" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="J255" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K255" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="L255" s="3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
     </row>
     <row r="256" spans="1:12" ht="13" customHeight="1">
       <c r="A256" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B256" s="13">
         <v>3</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="D256" s="13"/>
       <c r="E256" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F256" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="G256" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="H256" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I256" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="J256" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="K256" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="L256" s="3" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
     </row>
     <row r="257" spans="1:21" ht="13" customHeight="1">
       <c r="A257" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B257" s="13">
         <v>4</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D257" s="13"/>
       <c r="E257" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F257" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="G257" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="H257" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I257" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="J257" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="K257" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="L257" s="3" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
     </row>
     <row r="258" spans="1:21" ht="13" customHeight="1">
       <c r="A258" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="B258" s="13">
         <v>-99</v>
@@ -14473,13 +14473,13 @@
     </row>
     <row r="259" spans="1:21" ht="13" customHeight="1">
       <c r="A259" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B259" s="13">
         <v>0</v>
       </c>
       <c r="C259" s="13" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="D259" s="13"/>
       <c r="E259" s="13"/>
@@ -14493,13 +14493,13 @@
     </row>
     <row r="260" spans="1:21" ht="13" customHeight="1">
       <c r="A260" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B260" s="13">
         <v>1</v>
       </c>
       <c r="C260" s="13" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="D260" s="13"/>
       <c r="E260" s="13"/>
@@ -14513,13 +14513,13 @@
     </row>
     <row r="261" spans="1:21" ht="13" customHeight="1">
       <c r="A261" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B261" s="13">
         <v>2</v>
       </c>
       <c r="C261" s="13" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="D261" s="13"/>
       <c r="E261" s="13"/>
@@ -14533,13 +14533,13 @@
     </row>
     <row r="262" spans="1:21" ht="13" customHeight="1">
       <c r="A262" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B262" s="13">
         <v>3</v>
       </c>
       <c r="C262" s="13" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="D262" s="13"/>
       <c r="E262" s="13"/>
@@ -14553,13 +14553,13 @@
     </row>
     <row r="263" spans="1:21" ht="13" customHeight="1">
       <c r="A263" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B263" s="13">
         <v>4</v>
       </c>
       <c r="C263" s="13" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D263" s="13"/>
       <c r="E263" s="13"/>
@@ -14573,13 +14573,13 @@
     </row>
     <row r="264" spans="1:21" ht="13" customHeight="1">
       <c r="A264" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B264" s="13">
         <v>5</v>
       </c>
       <c r="C264" s="13" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="D264" s="13"/>
       <c r="E264" s="13"/>
@@ -14593,13 +14593,13 @@
     </row>
     <row r="265" spans="1:21" ht="13" customHeight="1">
       <c r="A265" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B265" s="13">
         <v>6</v>
       </c>
       <c r="C265" s="13" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="D265" s="13"/>
       <c r="E265" s="13"/>
@@ -14613,13 +14613,13 @@
     </row>
     <row r="266" spans="1:21" ht="13" customHeight="1">
       <c r="A266" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B266" s="13">
         <v>7</v>
       </c>
       <c r="C266" s="13" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="D266" s="13"/>
       <c r="E266" s="13"/>
@@ -14633,13 +14633,13 @@
     </row>
     <row r="267" spans="1:21" ht="13" customHeight="1">
       <c r="A267" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B267" s="13">
         <v>8</v>
       </c>
       <c r="C267" s="13" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="D267" s="13"/>
       <c r="E267" s="13"/>
@@ -14653,13 +14653,13 @@
     </row>
     <row r="268" spans="1:21" ht="13" customHeight="1">
       <c r="A268" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B268" s="13">
         <v>9</v>
       </c>
       <c r="C268" s="13" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="D268" s="13"/>
       <c r="E268" s="13"/>
@@ -14673,13 +14673,13 @@
     </row>
     <row r="269" spans="1:21" ht="13" customHeight="1">
       <c r="A269" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B269" s="13">
         <v>10</v>
       </c>
       <c r="C269" s="13" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="D269" s="13"/>
       <c r="E269" s="13"/>
@@ -14693,13 +14693,13 @@
     </row>
     <row r="270" spans="1:21" ht="13" customHeight="1">
       <c r="A270" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B270" s="13">
         <v>11</v>
       </c>
       <c r="C270" s="13" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="D270" s="13"/>
       <c r="E270" s="13"/>
@@ -14713,7 +14713,7 @@
     </row>
     <row r="271" spans="1:21" ht="13" customHeight="1">
       <c r="A271" s="13" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="B271" s="13">
         <v>-88</v>
@@ -14733,38 +14733,38 @@
     </row>
     <row r="272" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A272" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B272" s="25" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C272" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D272" s="25"/>
       <c r="E272" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="F272" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G272" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H272" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="I272" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="J272" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="K272" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="L272" s="25" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="M272" s="30"/>
       <c r="N272" s="30"/>
@@ -14778,38 +14778,38 @@
     </row>
     <row r="273" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A273" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B273" s="25" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C273" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="D273" s="25"/>
       <c r="E273" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="F273" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="G273" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H273" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="I273" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="J273" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="K273" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="L273" s="25" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="M273" s="30"/>
       <c r="N273" s="30"/>
@@ -14823,38 +14823,38 @@
     </row>
     <row r="274" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A274" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B274" s="25" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="C274" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D274" s="37"/>
       <c r="E274" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F274" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="G274" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H274" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="I274" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="J274" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="K274" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="L274" s="37" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="M274" s="30"/>
       <c r="N274" s="30"/>
@@ -14868,38 +14868,38 @@
     </row>
     <row r="275" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A275" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B275" s="25" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="C275" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="D275" s="37"/>
       <c r="E275" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F275" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="G275" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H275" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="I275" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="J275" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="K275" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L275" s="37" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="M275" s="30"/>
       <c r="N275" s="30"/>
@@ -14913,38 +14913,38 @@
     </row>
     <row r="276" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A276" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B276" s="25" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C276" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="D276" s="37"/>
       <c r="E276" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="F276" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="G276" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H276" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="I276" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="J276" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="K276" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="L276" s="37" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="M276" s="30"/>
       <c r="N276" s="30"/>
@@ -14958,38 +14958,38 @@
     </row>
     <row r="277" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A277" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B277" s="25" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="C277" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D277" s="37"/>
       <c r="E277" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F277" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="G277" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H277" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="I277" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="J277" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="K277" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="L277" s="37" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="M277" s="30"/>
       <c r="N277" s="30"/>
@@ -15003,38 +15003,38 @@
     </row>
     <row r="278" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A278" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B278" s="25" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C278" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D278" s="37"/>
       <c r="E278" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F278" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="G278" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H278" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="I278" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="J278" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="K278" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="L278" s="37" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="M278" s="30"/>
       <c r="N278" s="30"/>
@@ -15048,38 +15048,38 @@
     </row>
     <row r="279" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A279" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B279" s="25" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="C279" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D279" s="37"/>
       <c r="E279" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F279" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="G279" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H279" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="I279" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="J279" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="K279" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="L279" s="37" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="M279" s="30"/>
       <c r="N279" s="30"/>
@@ -15093,38 +15093,38 @@
     </row>
     <row r="280" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A280" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B280" s="25" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="C280" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D280" s="37"/>
       <c r="E280" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F280" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="G280" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H280" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="I280" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="J280" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="K280" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="L280" s="37" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="M280" s="30"/>
       <c r="N280" s="30"/>
@@ -15138,7 +15138,7 @@
     </row>
     <row r="281" spans="1:21" s="9" customFormat="1" ht="13" customHeight="1">
       <c r="A281" s="25" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B281" s="25" t="s">
         <v>102</v>
@@ -15220,30 +15220,30 @@
         <v>257</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="14" customFormat="1" ht="70">
       <c r="A2" s="32" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D2" s="18" t="b">
         <v>1</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
   </sheetData>
@@ -15278,22 +15278,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="22" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B1" s="23" t="s">
         <v>22</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -15304,16 +15304,16 @@
         <v>42796</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E2" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -15324,16 +15324,16 @@
         <v>42822</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -15344,16 +15344,16 @@
         <v>42829</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -15364,16 +15364,16 @@
         <v>42829</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E5" s="13" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -15384,16 +15384,16 @@
         <v>42829</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F6" s="25" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -15404,13 +15404,13 @@
         <v>42859</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -15421,16 +15421,16 @@
         <v>42890</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -15441,16 +15441,16 @@
         <v>42890</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -15461,16 +15461,16 @@
         <v>42920</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -15481,16 +15481,16 @@
         <v>42920</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -15501,16 +15501,16 @@
         <v>42920</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -15521,16 +15521,16 @@
         <v>42920</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -15541,16 +15541,16 @@
         <v>42951</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D14" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -15561,16 +15561,16 @@
         <v>42826</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -15581,16 +15581,16 @@
         <v>42847</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="24" spans="1:6">

</xml_diff>